<commit_message>
add stream name(utf8) to proto and config
</commit_message>
<xml_diff>
--- a/tools/xlsx2xml/xlsx/LocalServer/StreamSrcProxyConfig.xlsx
+++ b/tools/xlsx2xml/xlsx/LocalServer/StreamSrcProxyConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20340" windowHeight="7395"/>
+    <workbookView windowWidth="25320" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="StreamSrcProxyConfig" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
   <si>
     <t>ID</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Rate</t>
   </si>
   <si>
+    <t>SrcName</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -49,6 +52,9 @@
     <t>rtmp://193.112.189.182:1935/live/stream101</t>
   </si>
   <si>
+    <t>远程视频1</t>
+  </si>
+  <si>
     <t>远程视频推流</t>
   </si>
   <si>
@@ -58,33 +64,60 @@
     <t>rtmp://193.112.189.182:1935/live/stream102</t>
   </si>
   <si>
+    <t>远程视频2</t>
+  </si>
+  <si>
     <t>rtsp://192.168.1.100/13</t>
   </si>
   <si>
     <t>rtmp://193.112.189.182:1935/live/stream103</t>
   </si>
   <si>
+    <t>远程视频3</t>
+  </si>
+  <si>
     <t>rtsp://192.168.1.100/14</t>
   </si>
   <si>
     <t>rtmp://193.112.189.183:1935/live/stream104</t>
   </si>
   <si>
+    <t>远程视频4</t>
+  </si>
+  <si>
     <t>Local</t>
   </si>
   <si>
+    <t>本地视频1</t>
+  </si>
+  <si>
     <t>本地视频源</t>
   </si>
   <si>
+    <t>本地视频2</t>
+  </si>
+  <si>
+    <t>本地视频3</t>
+  </si>
+  <si>
+    <t>本地视频4</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
     <t>rtmp://193.112.189.183:1935/live/streamaudio</t>
   </si>
   <si>
+    <t>远程音频1</t>
+  </si>
+  <si>
     <t>远程音频推流</t>
   </si>
   <si>
+    <t>本地音频1</t>
+  </si>
+  <si>
     <t>本地音频源</t>
   </si>
   <si>
@@ -95,6 +128,9 @@
   </si>
   <si>
     <t>rtmp://193.112.189.183:1935/live/streamAV</t>
+  </si>
+  <si>
+    <t>远程音视频1</t>
   </si>
 </sst>
 </file>
@@ -102,10 +138,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -117,22 +153,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -147,21 +190,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -175,29 +242,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -214,6 +258,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -223,6 +274,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -231,32 +290,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -269,19 +305,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,163 +485,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,23 +513,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,11 +558,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,8 +591,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -568,10 +604,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -580,133 +616,133 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1033,25 +1069,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="10.875" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="17.75" customWidth="1"/>
     <col min="4" max="4" width="30.75" customWidth="1"/>
     <col min="5" max="5" width="46.625" customWidth="1"/>
-    <col min="6" max="6" width="18.125" customWidth="1"/>
-    <col min="7" max="7" width="24.25" customWidth="1"/>
-    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="6" max="7" width="18.125" customWidth="1"/>
+    <col min="8" max="8" width="24.25" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1073,208 +1109,240 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="1" spans="1:7">
+    <row r="6" customFormat="1" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6"/>
+        <v>10</v>
+      </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="7" customFormat="1" spans="1:7">
+    <row r="7" customFormat="1" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7"/>
+        <v>14</v>
+      </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="1" spans="1:7">
+    <row r="8" customFormat="1" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8"/>
+        <v>17</v>
+      </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="9" customFormat="1" spans="1:7">
+    <row r="9" customFormat="1" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9"/>
+        <v>20</v>
+      </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F11">
         <v>16000</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>